<commit_message>
Cleaned up results logging. Added number of jobs to run definition to model. Fixed buffer capacity to accept 2 chars. Created clean dataCrawler module for process discovery information.
</commit_message>
<xml_diff>
--- a/ASAE/EventLog.xlsx
+++ b/ASAE/EventLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="108">
   <si>
     <t>JobID Start</t>
   </si>
@@ -40,337 +40,304 @@
     <t>1</t>
   </si>
   <si>
-    <t>[1:1-(x)]</t>
+    <t>1.003956</t>
+  </si>
+  <si>
+    <t>[2:0-(x)]</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>1.003956</t>
-  </si>
-  <si>
-    <t>[2:0-(x)]</t>
+    <t>[1:1-([1:0-(x)])]</t>
+  </si>
+  <si>
+    <t>1.003991</t>
+  </si>
+  <si>
+    <t>2.516865</t>
+  </si>
+  <si>
+    <t>[3:0-(x)]</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>1.512909</t>
-  </si>
-  <si>
-    <t>[2:1-(x)]</t>
+    <t>4.474623</t>
+  </si>
+  <si>
+    <t>[4:0-(x)]</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>[1:2-([1:1-(x)][1:0-(x)])]</t>
-  </si>
-  <si>
-    <t>1.513026</t>
-  </si>
-  <si>
-    <t>3.304822</t>
-  </si>
-  <si>
-    <t>[3:0-(x)]</t>
+    <t>6.507946</t>
+  </si>
+  <si>
+    <t>[5:0-(x)]</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>3.470667</t>
-  </si>
-  <si>
-    <t>[3:1-(x)]</t>
+    <t>8.169700</t>
+  </si>
+  <si>
+    <t>[6:0-(x)]</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>4.777407</t>
-  </si>
-  <si>
-    <t>[4:1-(x)]</t>
+    <t>9.476439</t>
+  </si>
+  <si>
+    <t>[7:0-(x)]</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>4.966576</t>
-  </si>
-  <si>
-    <t>[4:0-(x)]</t>
+    <t>10.304856</t>
+  </si>
+  <si>
+    <t>[2:1-([2:0-(x)])]</t>
+  </si>
+  <si>
+    <t>[1:2-([1:1-([1:0-(x)])])]</t>
+  </si>
+  <si>
+    <t>10.305534</t>
+  </si>
+  <si>
+    <t>11.675022</t>
+  </si>
+  <si>
+    <t>[8:0-(x)]</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>6.975989</t>
-  </si>
-  <si>
-    <t>[5:1-(x)]</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>7.165697</t>
-  </si>
-  <si>
-    <t>[5:0-(x)]</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>7.546349</t>
-  </si>
-  <si>
-    <t>[2:2-([2:1-(x)][2:0-(x)])]</t>
-  </si>
-  <si>
-    <t>9.041485</t>
-  </si>
-  <si>
-    <t>[6:0-(x)]</t>
-  </si>
-  <si>
-    <t>9.614583</t>
-  </si>
-  <si>
-    <t>[6:1-(x)]</t>
-  </si>
-  <si>
-    <t>10.877536</t>
-  </si>
-  <si>
-    <t>[7:1-(x)]</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>11.460048</t>
-  </si>
-  <si>
-    <t>[7:0-(x)]</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>12.204527</t>
-  </si>
-  <si>
-    <t>[8:1-(x)]</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>13.490203</t>
-  </si>
-  <si>
-    <t>[8:0-(x)]</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>13.565957</t>
-  </si>
-  <si>
-    <t>[3:2-([3:1-(x)][3:0-(x)])]</t>
-  </si>
-  <si>
-    <t>14.393539</t>
-  </si>
-  <si>
-    <t>[9:1-(x)]</t>
-  </si>
-  <si>
-    <t>14.614285</t>
+    <t>12.944128</t>
+  </si>
+  <si>
+    <t>13.550810</t>
+  </si>
+  <si>
+    <t>19.503979</t>
+  </si>
+  <si>
+    <t>[3:1-([3:0-(x)])]</t>
+  </si>
+  <si>
+    <t>[2:2-([2:1-([2:0-(x)])])]</t>
+  </si>
+  <si>
+    <t>19.504436</t>
   </si>
   <si>
     <t>[9:0-(x)]</t>
   </si>
   <si>
-    <t>15.759169</t>
-  </si>
-  <si>
-    <t>16.528053</t>
-  </si>
-  <si>
-    <t>19.441647</t>
-  </si>
-  <si>
-    <t>[4:2-([4:1-(x)][4:0-(x)])]</t>
-  </si>
-  <si>
-    <t>[10:1-(x)]</t>
-  </si>
-  <si>
-    <t>19.441763</t>
+    <t>19.504873</t>
+  </si>
+  <si>
+    <t>20.767826</t>
+  </si>
+  <si>
+    <t>21.922998</t>
+  </si>
+  <si>
+    <t>28.523586</t>
+  </si>
+  <si>
+    <t>[4:1-([4:0-(x)])]</t>
+  </si>
+  <si>
+    <t>[3:2-([3:1-([3:0-(x)])])]</t>
+  </si>
+  <si>
+    <t>28.524370</t>
   </si>
   <si>
     <t>[10:0-(x)]</t>
   </si>
   <si>
-    <t>19.441805</t>
-  </si>
-  <si>
-    <t>21.535095</t>
-  </si>
-  <si>
-    <t>22.068808</t>
-  </si>
-  <si>
-    <t>25.650158</t>
-  </si>
-  <si>
-    <t>[5:2-([5:1-(x)][5:0-(x)])]</t>
+    <t>28.524563</t>
+  </si>
+  <si>
+    <t>30.554525</t>
+  </si>
+  <si>
+    <t>30.713575</t>
+  </si>
+  <si>
+    <t>36.850578</t>
+  </si>
+  <si>
+    <t>[5:1-([5:0-(x)])]</t>
+  </si>
+  <si>
+    <t>[4:2-([4:1-([4:0-(x)])])]</t>
+  </si>
+  <si>
+    <t>36.851067</t>
   </si>
   <si>
     <t>[11:0-(x)]</t>
   </si>
   <si>
-    <t>25.650265</t>
-  </si>
-  <si>
-    <t>[11:1-(x)]</t>
-  </si>
-  <si>
-    <t>25.650276</t>
-  </si>
-  <si>
-    <t>27.079147</t>
-  </si>
-  <si>
-    <t>27.677567</t>
-  </si>
-  <si>
-    <t>32.095482</t>
-  </si>
-  <si>
-    <t>[6:2-([6:1-(x)][6:0-(x)])]</t>
-  </si>
-  <si>
-    <t>[12:1-(x)]</t>
-  </si>
-  <si>
-    <t>32.095631</t>
+    <t>36.851204</t>
+  </si>
+  <si>
+    <t>38.216831</t>
+  </si>
+  <si>
+    <t>38.726757</t>
+  </si>
+  <si>
+    <t>44.974663</t>
+  </si>
+  <si>
+    <t>[6:1-([6:0-(x)])]</t>
   </si>
   <si>
     <t>[12:0-(x)]</t>
   </si>
   <si>
-    <t>32.095638</t>
-  </si>
-  <si>
-    <t>34.007771</t>
-  </si>
-  <si>
-    <t>34.322578</t>
-  </si>
-  <si>
-    <t>38.263519</t>
-  </si>
-  <si>
-    <t>[7:2-([7:1-(x)][7:0-(x)])]</t>
-  </si>
-  <si>
-    <t>[13:1-(x)]</t>
-  </si>
-  <si>
-    <t>38.263676</t>
+    <t>44.975117</t>
+  </si>
+  <si>
+    <t>[5:2-([5:1-([5:0-(x)])])]</t>
+  </si>
+  <si>
+    <t>44.975323</t>
+  </si>
+  <si>
+    <t>47.068653</t>
+  </si>
+  <si>
+    <t>47.183628</t>
+  </si>
+  <si>
+    <t>53.888432</t>
+  </si>
+  <si>
+    <t>[7:1-([7:0-(x)])]</t>
+  </si>
+  <si>
+    <t>[6:2-([6:1-([6:0-(x)])])]</t>
+  </si>
+  <si>
+    <t>53.888905</t>
   </si>
   <si>
     <t>[13:0-(x)]</t>
   </si>
   <si>
-    <t>38.263680</t>
-  </si>
-  <si>
-    <t>39.988182</t>
-  </si>
-  <si>
-    <t>40.574036</t>
-  </si>
-  <si>
-    <t>44.840012</t>
-  </si>
-  <si>
-    <t>[8:2-([8:1-(x)][8:0-(x)])]</t>
-  </si>
-  <si>
-    <t>[14:1-(x)]</t>
-  </si>
-  <si>
-    <t>44.840057</t>
+    <t>53.888943</t>
+  </si>
+  <si>
+    <t>55.916245</t>
+  </si>
+  <si>
+    <t>56.334229</t>
+  </si>
+  <si>
+    <t>63.515434</t>
+  </si>
+  <si>
+    <t>[8:1-([8:0-(x)])]</t>
   </si>
   <si>
     <t>[14:0-(x)]</t>
   </si>
   <si>
-    <t>44.840172</t>
-  </si>
-  <si>
-    <t>46.650398</t>
-  </si>
-  <si>
-    <t>47.113533</t>
-  </si>
-  <si>
-    <t>50.148117</t>
-  </si>
-  <si>
-    <t>[9:2-([9:1-(x)][9:0-(x)])]</t>
+    <t>63.516068</t>
+  </si>
+  <si>
+    <t>[7:2-([7:1-([7:0-(x)])])]</t>
+  </si>
+  <si>
+    <t>63.516281</t>
+  </si>
+  <si>
+    <t>65.428421</t>
+  </si>
+  <si>
+    <t>65.684105</t>
+  </si>
+  <si>
+    <t>71.944305</t>
+  </si>
+  <si>
+    <t>[9:1-([9:0-(x)])]</t>
   </si>
   <si>
     <t>[15:0-(x)]</t>
   </si>
   <si>
-    <t>50.148155</t>
-  </si>
-  <si>
-    <t>[15:1-(x)]</t>
-  </si>
-  <si>
-    <t>50.148308</t>
-  </si>
-  <si>
-    <t>52.450172</t>
-  </si>
-  <si>
-    <t>53.014423</t>
-  </si>
-  <si>
-    <t>56.290958</t>
-  </si>
-  <si>
-    <t>[10:2-([10:1-(x)][10:0-(x)])]</t>
-  </si>
-  <si>
-    <t>[16:1-(x)]</t>
-  </si>
-  <si>
-    <t>56.291004</t>
+    <t>71.944664</t>
+  </si>
+  <si>
+    <t>[8:2-([8:1-([8:0-(x)])])]</t>
+  </si>
+  <si>
+    <t>71.944839</t>
+  </si>
+  <si>
+    <t>74.255196</t>
+  </si>
+  <si>
+    <t>74.521156</t>
+  </si>
+  <si>
+    <t>81.171249</t>
+  </si>
+  <si>
+    <t>[10:1-([10:0-(x)])]</t>
+  </si>
+  <si>
+    <t>[9:2-([9:1-([9:0-(x)])])]</t>
+  </si>
+  <si>
+    <t>81.171394</t>
   </si>
   <si>
     <t>[16:0-(x)]</t>
   </si>
   <si>
-    <t>56.291100</t>
-  </si>
-  <si>
-    <t>57.993912</t>
-  </si>
-  <si>
-    <t>59.104286</t>
-  </si>
-  <si>
-    <t>62.145756</t>
+    <t>81.171501</t>
+  </si>
+  <si>
+    <t>82.479500</t>
+  </si>
+  <si>
+    <t>83.444977</t>
+  </si>
+  <si>
+    <t>89.895752</t>
+  </si>
+  <si>
+    <t>[11:1-([11:0-(x)])]</t>
+  </si>
+  <si>
+    <t>[10:2-([10:1-([10:0-(x)])])]</t>
+  </si>
+  <si>
+    <t>89.896423</t>
+  </si>
+  <si>
+    <t>[17:0-(x)]</t>
+  </si>
+  <si>
+    <t>89.896431</t>
+  </si>
+  <si>
+    <t>92.039261</t>
   </si>
 </sst>
 </file>
@@ -702,7 +669,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -742,30 +709,30 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -773,16 +740,16 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
@@ -799,173 +766,173 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
       <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
         <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -973,19 +940,19 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
         <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -993,59 +960,59 @@
         <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
         <v>51</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G17" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1053,39 +1020,39 @@
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G18" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G19" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1093,19 +1060,19 @@
         <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
         <v>60</v>
       </c>
       <c r="G20" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1113,39 +1080,39 @@
         <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F21" t="s">
         <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F22" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G22" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1153,59 +1120,59 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F23" t="s">
         <v>68</v>
       </c>
       <c r="G23" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F24" t="s">
         <v>69</v>
       </c>
       <c r="G24" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G25" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1213,59 +1180,59 @@
         <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F26" t="s">
         <v>76</v>
       </c>
       <c r="G26" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F27" t="s">
         <v>77</v>
       </c>
       <c r="G27" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F28" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G28" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1273,59 +1240,59 @@
         <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F29" t="s">
         <v>84</v>
       </c>
       <c r="G29" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F30" t="s">
         <v>85</v>
       </c>
       <c r="G30" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="F31" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="G31" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1333,59 +1300,59 @@
         <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F32" t="s">
         <v>92</v>
       </c>
       <c r="G32" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F33" t="s">
         <v>93</v>
       </c>
       <c r="G33" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E34" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="F34" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G34" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1393,59 +1360,59 @@
         <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F35" t="s">
         <v>100</v>
       </c>
       <c r="G35" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F36" t="s">
         <v>101</v>
       </c>
       <c r="G36" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="F37" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G37" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1453,119 +1420,21 @@
         <v>103</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" t="s">
-        <v>104</v>
-      </c>
-      <c r="F38" t="s">
-        <v>108</v>
-      </c>
-      <c r="G38" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" t="s">
-        <v>106</v>
-      </c>
-      <c r="F39" t="s">
-        <v>109</v>
-      </c>
-      <c r="G39" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" t="s">
-        <v>106</v>
-      </c>
-      <c r="B40" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" t="s">
-        <v>103</v>
-      </c>
-      <c r="F40" t="s">
-        <v>110</v>
-      </c>
-      <c r="G40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" t="s">
-        <v>110</v>
-      </c>
-      <c r="C41" t="s">
-        <v>47</v>
-      </c>
-      <c r="E41" t="s">
-        <v>112</v>
-      </c>
-      <c r="F41" t="s">
-        <v>116</v>
-      </c>
-      <c r="G41" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" t="s">
-        <v>112</v>
-      </c>
-      <c r="B42" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" t="s">
-        <v>50</v>
-      </c>
-      <c r="E42" t="s">
-        <v>114</v>
-      </c>
-      <c r="F42" t="s">
-        <v>117</v>
-      </c>
-      <c r="G42" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" t="s">
-        <v>114</v>
-      </c>
-      <c r="B43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C43" t="s">
-        <v>53</v>
-      </c>
-      <c r="E43" t="s">
-        <v>111</v>
-      </c>
-      <c r="F43" t="s">
-        <v>118</v>
-      </c>
-      <c r="G43" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>